<commit_message>
update data load page
</commit_message>
<xml_diff>
--- a/data/input/sample_mev_data.xlsx
+++ b/data/input/sample_mev_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himan\Desktop\TSA\time-series-analysis\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DFFDC8-590B-43A2-B461-181CDD9D6E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47353A63-26BF-48E2-8F01-BBEC4733500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{216A00CD-6235-43AA-BD44-0304FB0FF6D1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Macro Variable</t>
   </si>
@@ -47,13 +47,31 @@
     <t>Description</t>
   </si>
   <si>
-    <t>GDP</t>
-  </si>
-  <si>
     <t>201003-201312</t>
   </si>
   <si>
     <t>Gross Domestic Product</t>
+  </si>
+  <si>
+    <t>gdp</t>
+  </si>
+  <si>
+    <t>cpi</t>
+  </si>
+  <si>
+    <t>int_rt</t>
+  </si>
+  <si>
+    <t>s_p_index</t>
+  </si>
+  <si>
+    <t>Consumer Price Index</t>
+  </si>
+  <si>
+    <t>Interest Rate</t>
+  </si>
+  <si>
+    <t>S &amp; P Index</t>
   </si>
 </sst>
 </file>
@@ -425,167 +443,338 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8FFBF5-B642-4792-9F55-C1ECC0F4D110}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>201003</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>201006</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>201009</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>201012</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>201103</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>201106</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>201109</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>201112</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>201203</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>201206</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>201209</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>201212</v>
       </c>
       <c r="B15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>201303</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>201306</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>201309</v>
       </c>
       <c r="B18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>201312</v>
       </c>
       <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
         <v>6</v>
       </c>
     </row>

</xml_diff>